<commit_message>
Finished Quiz  includes old quiz junk
</commit_message>
<xml_diff>
--- a/Quiz/QuizSetupSpreadsheet.xlsx
+++ b/Quiz/QuizSetupSpreadsheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Problem Type</t>
   </si>
@@ -93,15 +93,6 @@
     <t>What was Daniel Bernoulli’s major contribution to our understanding of water power?</t>
   </si>
   <si>
-    <t>C:\Users\NIK12\Desktop\Question2.png</t>
-  </si>
-  <si>
-    <t>C:\Users\NIK12\Desktop\Question3.png</t>
-  </si>
-  <si>
-    <t>C:\Users\NIK12\Desktop\Question4.png</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -112,6 +103,45 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>C:\Users\husmith\Documents\GitHub\Action Pack\Quiz\Question2.png</t>
+  </si>
+  <si>
+    <t>C:\Users\husmith\Documents\GitHub\Action Pack\Quiz\Question1.png</t>
+  </si>
+  <si>
+    <t>C:\Users\husmith\Documents\GitHub\Action Pack\Quiz\Question3.png</t>
+  </si>
+  <si>
+    <t>Text &amp; Image</t>
+  </si>
+  <si>
+    <t>Whats the Deal?</t>
+  </si>
+  <si>
+    <t>SelectMulti</t>
+  </si>
+  <si>
+    <t>What?</t>
+  </si>
+  <si>
+    <t>Who</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>Ship</t>
+  </si>
+  <si>
+    <t>Holla at ya boy!</t>
+  </si>
+  <si>
+    <t>True/False</t>
+  </si>
+  <si>
+    <t>Flase</t>
   </si>
 </sst>
 </file>
@@ -811,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -922,13 +952,13 @@
       <c r="K2" s="8"/>
       <c r="U2" s="16"/>
     </row>
-    <row r="3" spans="1:21" ht="45">
+    <row r="3" spans="1:21" ht="75">
       <c r="A3" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="13" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>22</v>
@@ -936,29 +966,29 @@
       <c r="E3" s="8"/>
       <c r="I3" s="8"/>
       <c r="K3" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L3" s="27" t="b">
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="U3" s="16"/>
     </row>
-    <row r="4" spans="1:21" ht="45">
+    <row r="4" spans="1:21" ht="75">
       <c r="A4" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="13" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>22</v>
@@ -966,29 +996,29 @@
       <c r="E4" s="8"/>
       <c r="I4" s="8"/>
       <c r="K4" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L4" s="27" t="b">
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="U4" s="16"/>
     </row>
-    <row r="5" spans="1:21" ht="45">
+    <row r="5" spans="1:21" ht="75">
       <c r="A5" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="13" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>2</v>
@@ -999,22 +1029,55 @@
       <c r="U5" s="16"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="B6" s="2"/>
+      <c r="A6" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="C6" s="13"/>
-      <c r="D6" s="15"/>
+      <c r="D6" s="15" t="s">
+        <v>34</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="K6" s="8"/>
+      <c r="K6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>38</v>
+      </c>
       <c r="U6" s="16"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="B7" s="2"/>
+      <c r="A7" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C7" s="13"/>
-      <c r="D7" s="15"/>
+      <c r="D7" s="15" t="s">
+        <v>40</v>
+      </c>
       <c r="E7" s="8"/>
       <c r="I7" s="8"/>
       <c r="K7" s="8"/>
-      <c r="U7" s="16"/>
+      <c r="U7" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:21">
       <c r="B8" s="2"/>
@@ -1234,14 +1297,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
       <formula1>"Text, Text &amp; Image, Image"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H27:H1048576 G1:G26 K27:K1048576 J1:J26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H27:H1048576 J1:J26 K27:K1048576 G1:G26">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I27:I1048576 H1:H26">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M27:M1048576 N1:N26 P1:P26 R1:R26 T1:T26 L1:L26 U27:U1048576 S27:S1048576 Q27:Q1048576 O27:O1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M27:M1048576 O27:O1048576 Q27:Q1048576 S27:S1048576 U27:U1048576 L1:L26 T1:T26 R1:R26 P1:P26 N1:N26">
       <formula1>"True, False"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U26">

</xml_diff>